<commit_message>
feat: add auto send message
</commit_message>
<xml_diff>
--- a/input/汇总_资源.xlsx
+++ b/input/汇总_资源.xlsx
@@ -1835,36 +1835,34 @@
     <row r="33" ht="25.5" customHeight="1">
       <c r="A33" t="inlineStr">
         <is>
-          <t>【职规赛专属PPT模</t>
+          <t>高品质400+简历模</t>
         </is>
       </c>
       <c r="B33">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>【职规赛专属PPT模板（夺冠必备版）】
-让职业规划演示页间衔接流畅自然，瞬间提升答辩专业度与吸睛度～
-模板覆盖自我认知、职业分析、路径规划、实施计划等职规赛核心模块，从初赛到决赛的全阶段展示场景都能精准适配～更高效实用，可一键替换数据图表与个人案例，灵活匹配不同专业方向的内容需求～
-设计简约大气，重点内容排版突出，文字、数据、图表编辑替换超便捷，零设计基础也能快速打造符合评审偏好的高水准答辩PPT！
-超省心冲刺职规赛高分
-全模块覆盖+一键编辑，适配不同专业答辩需求
-网盘，拍下即发，助力快速完成演示准备
-【免责声明】
-文件均来自公开网络资源，仅供学习和交流，版权归原作者所有。如有版权问题，请及时联系我们删除。商品价格仅代表资源查找和整理的劳动成本，支持正版。本店商品仅限个人学习使用，不涉及商业用途。
-</t>
+          <t>高品质400+简历模板个人求职电子版word封面应届毕业生表格英文设计制作定制
+——★24小时自动秒发百度网盘 ★——
+预览图对应相应源文件名字，不是卖图片，也没有任何额外费用，如果不会使用可以咨询解决[送花][送花][送花]
+拍下直接发400套高质量简历模板
+单页，双页，四页，多页均有，自荐信模版，英文版，多种模板，任你选择
+可以用手机直接编辑哦
+不要问在不在，喜欢的直接拍下即可！秒发
+您想要的各种素材都在这里 任何不满意直接退款</t>
         </is>
       </c>
       <c r="F33" s="2" t="str">
-        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i1/O1CN01gJCxys1IFlIBxegEk_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i1/O1CN01gJCxys1IFlIBxegEk_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp")</f>
-        <v>img.alicdn.com/bao/uploaded/i1/O1CN01gJCxys1IFlIBxegEk_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp</v>
+        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i2/O1CN01XvG7871dZ5w9EjfQX_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i2/O1CN01XvG7871dZ5w9EjfQX_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp")</f>
+        <v>img.alicdn.com/bao/uploaded/i2/O1CN01XvG7871dZ5w9EjfQX_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp</v>
       </c>
       <c r="G33"/>
       <c r="H33" s="2" t="str">
-        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.137.69b752f39oihHY&amp;id=978499846717&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.137.69b752f39oihHY&amp;id=978499846717&amp;categoryId=50023914")</f>
-        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.137.69b752f39oihHY&amp;id=978499846717&amp;categoryId=50023914</v>
+        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.295.12e16ac2PYxLX9&amp;id=750009782412&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.295.12e16ac2PYxLX9&amp;id=750009782412&amp;categoryId=50023914")</f>
+        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.295.12e16ac2PYxLX9&amp;id=750009782412&amp;categoryId=50023914</v>
       </c>
       <c r="I33"/>
       <c r="J33"/>
@@ -1873,43 +1871,37 @@
     <row r="34" ht="25.5" customHeight="1">
       <c r="A34" t="inlineStr">
         <is>
-          <t>毕业论文技术路线图模</t>
+          <t>科研PPT模板学术汇</t>
         </is>
       </c>
       <c r="B34">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34" t="inlineStr">
         <is>
-          <t>毕业论文技术路线图模板合集（100+套精选）|||
-包含文件内容：
-1. 可编辑Word模板（30套）
-- 每套独立Word文件，含预览图展示
-- 直接编辑文字/图形，适配开题报告需求
-2. 高效整合版Word模板（50套）没有预览图可直接打开word查看
-- 集中收录于单一Word文档，快速浏览调用
-- 涵盖实验设计/理论研究/数据分析等多场景
-3. 专业Visio模板（17套）
-- VSDX格式源文件，需用Visio软件编辑
-- 支持复杂流程图、系统架构图等高阶需求
-格式说明：
-- 所有模板文字/图形可自由修改
-- （Visio需安装对应软件）
-交付方式：
-- 自动发链接，即时下载
-- 数字资源不支持退换</t>
+          <t>科研PPT模板学术汇报项目组会论文献答辩研究生开题报告职称申报
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+宝贝秒拍秒发，拍下全发！你想要各种素材都在这里 任何不满意直接退款！！！
+如果没有及时回复可以先拍下来看是否需要和满意，不满意没有需要直接退款即可，上线会立即处理，您放心。
+预览图对应相应源文件名字，不是卖图片，也没有任何额外费用，如果不会使用可以咨询解决
+每套风格的模版都是我精心挑选出来的。
+每款精选质量高，适用于任何场合～
+每个风格都有单独归类文档编号
+</t>
         </is>
       </c>
       <c r="F34" s="2" t="str">
-        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i4/O1CN01APm8jd1IFlH45LKPb_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i4/O1CN01APm8jd1IFlH45LKPb_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp")</f>
-        <v>img.alicdn.com/bao/uploaded/i4/O1CN01APm8jd1IFlH45LKPb_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp</v>
+        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i3/O1CN01aRdK1I1dZ5wmHoKdF_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i3/O1CN01aRdK1I1dZ5wmHoKdF_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp")</f>
+        <v>img.alicdn.com/bao/uploaded/i3/O1CN01aRdK1I1dZ5wmHoKdF_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp</v>
       </c>
       <c r="G34"/>
       <c r="H34" s="2" t="str">
-        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.76.69b752f39oihHY&amp;id=952820257064&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.76.69b752f39oihHY&amp;id=952820257064&amp;categoryId=50023914")</f>
-        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.76.69b752f39oihHY&amp;id=952820257064&amp;categoryId=50023914</v>
+        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.360.12e16ac2PYxLX9&amp;id=986502332050&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.360.12e16ac2PYxLX9&amp;id=986502332050&amp;categoryId=50023914")</f>
+        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.360.12e16ac2PYxLX9&amp;id=986502332050&amp;categoryId=50023914</v>
       </c>
       <c r="I34"/>
       <c r="J34"/>
@@ -1918,30 +1910,39 @@
     <row r="35" ht="25.5" customHeight="1">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025家装避坑全流</t>
+          <t>课题申报框架构图教学</t>
         </is>
       </c>
       <c r="B35">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2025家装避坑全流程资料包2025年家装避坑全流程指南 ！一站式购齐所有装修资料！
-拍下秒发25样全套全流程资料！家装大全电子档+装修全流程大全+装修避坑大全+装修小白必备+装修常用尺寸设计+装修合同模版+装修预算表+全屋效果图+全屋定制效果图+室内设计软装模版+施工流程及工艺要求+高端室内设计案例+装修验收标准+全屋插座定位图
-手机电脑都可以随时查看，非常齐全最新版本，直接下单即可。
-要求高的不要下单，而且卖掉0.01已经相当于免费送了</t>
+          <t>课题申报框架构图教学思政科研绘图技术路线图visoi流程图ppt模板
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+280款流程架构路线图 PPT + WORD +VISOI
+课题申报 教学大赛 技术路线 科研论文
+宝贝秒拍秒发，拍下全发！你想要各种素材都在这里 任何不满意直接退款！！！
+如果没有及时回复可以先拍下来看是否需要和满意，不满意没有需要直接退款即可，上线会立即处理，您放心。
+预览图对应相应源文件名字，不是卖图片，也没有任何额外费用，如果不会使用可以咨询解决
+每套风格的模版都是我精心挑选出来的。
+每款精选质量高，适用于任何场合～
+每个风格都有单独归类文档编号
+</t>
         </is>
       </c>
       <c r="F35" s="2" t="str">
-        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i1/O1CN015k8GWx1IFlGj3P9qF_!!4611686018427383856-0-fleamarket.jpg_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i1/O1CN015k8GWx1IFlGj3P9qF_!!4611686018427383856-0-fleamarket.jpg_790x10000Q90.jpg_.webp")</f>
-        <v>img.alicdn.com/bao/uploaded/i1/O1CN015k8GWx1IFlGj3P9qF_!!4611686018427383856-0-fleamarket.jpg_790x10000Q90.jpg_.webp</v>
+        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i1/O1CN01oQTUGX1dZ5wze9757_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i1/O1CN01oQTUGX1dZ5wze9757_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp")</f>
+        <v>img.alicdn.com/bao/uploaded/i1/O1CN01oQTUGX1dZ5wze9757_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp</v>
       </c>
       <c r="G35"/>
       <c r="H35" s="2" t="str">
-        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.37.69b752f39oihHY&amp;id=945646124837&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.37.69b752f39oihHY&amp;id=945646124837&amp;categoryId=50023914")</f>
-        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.37.69b752f39oihHY&amp;id=945646124837&amp;categoryId=50023914</v>
+        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.108.12e16ac2PYxLX9&amp;id=990745156115&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.108.12e16ac2PYxLX9&amp;id=990745156115&amp;categoryId=50023914")</f>
+        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.108.12e16ac2PYxLX9&amp;id=990745156115&amp;categoryId=50023914</v>
       </c>
       <c r="I35"/>
       <c r="J35"/>
@@ -1950,37 +1951,37 @@
     <row r="36" ht="25.5" customHeight="1">
       <c r="A36" t="inlineStr">
         <is>
-          <t>【秒发】领导超爱的高</t>
+          <t>大学生国家奖学金励志</t>
         </is>
       </c>
       <c r="B36">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>【秒发】领导超爱的高级感工作汇报PPT模版 逻辑图 数据图|||
-排版简洁干净，高端大气，打工人必备！
-九个模版九种配色 每套160页
-附赠：国外高端PPT模版（400p）、常用小图标、字体包
-由于电子教程的可复制性，发货后不得退款，敬请谅解！
-【免责声明】
-上架资源均由个人亲自整理 且标注免责声明以及对应图片 具体内容如下:
-1.所有文件均获取自网络公开渠道，仅供学习和交流使用，所有版权归版权人所有。
-2.如版权方认为侵犯了您的版权，请及时联系小店删除
-3.本店所有商品售价仅是对资源查找以及整理的加工费用，如喜欢作品，请支持正版哦~
-4.本店所有商品不涉及商用，仅是以众筹的于提供给想要学习的极少部分人用于学习。</t>
+          <t>大学生国家奖学金励志国奖答辩竞选PPT模板蓝红色主题大气高级感
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+宝贝秒拍秒发，拍下全发！你想要各种素材都在这里 任何不满意直接退款！！！
+如果没有及时回复可以先拍下来看是否需要和满意，不满意没有需要直接退款即可，上线会立即处理，您放心。
+预览图对应相应源文件名字，不是卖图片，也没有任何额外费用，如果不会使用可以咨询解决
+每套风格的模版都是我精心挑选出来的。
+每款精选质量高，适用于任何场合～
+每个风格都有单独归类文档编号
+</t>
         </is>
       </c>
       <c r="F36" s="2" t="str">
-        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i2/O1CN01XVcaDw1IFlGsPe3nG_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i2/O1CN01XVcaDw1IFlGsPe3nG_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp")</f>
-        <v>img.alicdn.com/bao/uploaded/i2/O1CN01XVcaDw1IFlGsPe3nG_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp</v>
+        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i2/O1CN014Sac8D1dZ5wncs34U_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i2/O1CN014Sac8D1dZ5wncs34U_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp")</f>
+        <v>img.alicdn.com/bao/uploaded/i2/O1CN014Sac8D1dZ5wncs34U_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="2" t="str">
-        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.8.69b752f39oihHY&amp;id=948022201397&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.8.69b752f39oihHY&amp;id=948022201397&amp;categoryId=50023914")</f>
-        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.8.69b752f39oihHY&amp;id=948022201397&amp;categoryId=50023914</v>
+        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.114.12e16ac2PYxLX9&amp;id=985828185520&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.114.12e16ac2PYxLX9&amp;id=985828185520&amp;categoryId=50023914")</f>
+        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.114.12e16ac2PYxLX9&amp;id=985828185520&amp;categoryId=50023914</v>
       </c>
       <c r="I36"/>
       <c r="J36"/>
@@ -1989,29 +1990,38 @@
     <row r="37" ht="25.5" customHeight="1">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Excel函数公式大</t>
+          <t>电商详情页psd模板</t>
         </is>
       </c>
       <c r="B37">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Excel函数公式大全精讲Excel函数公式大全总结（史上最强总结），例子简单明了！一|||共有5个excel文件，每个excel里面多个sheet表的内容，绝大部分函数都有。
-以下仅为部分资料截图
-感兴趣的小伙伴，点击我想要，然后点右上角立即购买后联系客服，文件以网盘的方式发给您！</t>
+          <t>电商详情页psd模板店铺装修设计主图美工背景促销海报源文件素材
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+5万款全套电商素材模板 主图 详情图 首页 店招 促销 标签
+宝贝秒拍秒发，拍下全发！你想要各种素材都在这里 任何不满意直接退款！！！
+如果没有及时回复可以先拍下来看是否需要和满意，不满意没有需要直接退款即可，上线会立即处理，您放心。
+预览图对应相应源文件名字，不是卖图片，也没有任何额外费用，如果不会使用可以咨询解决
+每套风格的模版都是我精心挑选出来的。
+每款精选质量高，适用于任何场合～
+每个风格都有单独归类文档编号
+</t>
         </is>
       </c>
       <c r="F37" s="2" t="str">
-        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i2/O1CN01jtIuMb1IFlH7nTboG_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i2/O1CN01jtIuMb1IFlH7nTboG_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp")</f>
-        <v>img.alicdn.com/bao/uploaded/i2/O1CN01jtIuMb1IFlH7nTboG_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp</v>
+        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i4/O1CN010gRoUm1dZ5x3WeSEi_!!4611686018427387605-2-fleamarket.png_790x10000.jpg_.webp", "img.alicdn.com/bao/uploaded/i4/O1CN010gRoUm1dZ5x3WeSEi_!!4611686018427387605-2-fleamarket.png_790x10000.jpg_.webp")</f>
+        <v>img.alicdn.com/bao/uploaded/i4/O1CN010gRoUm1dZ5x3WeSEi_!!4611686018427387605-2-fleamarket.png_790x10000.jpg_.webp</v>
       </c>
       <c r="G37"/>
       <c r="H37" s="2" t="str">
-        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.140.69b752f39oihHY&amp;id=954223364616&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.140.69b752f39oihHY&amp;id=954223364616&amp;categoryId=50023914")</f>
-        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.140.69b752f39oihHY&amp;id=954223364616&amp;categoryId=50023914</v>
+        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.365.12e16ac2PYxLX9&amp;id=989828106972&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.365.12e16ac2PYxLX9&amp;id=989828106972&amp;categoryId=50023914")</f>
+        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.365.12e16ac2PYxLX9&amp;id=989828106972&amp;categoryId=50023914</v>
       </c>
       <c r="I37"/>
       <c r="J37"/>
@@ -2020,27 +2030,37 @@
     <row r="38" ht="25.5" customHeight="1">
       <c r="A38" t="inlineStr">
         <is>
-          <t>（自动发货）289页</t>
+          <t>大学生职业生涯规划大</t>
         </is>
       </c>
       <c r="B38">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>（自动发货）289页高级PPT图文排版，领导看了直呼哇塞！支|||持一键换色，整版可编辑，多种配色方案。包含3图44页、4图48页、5图37页、6图50页、7图36页、8图35页、多图39页，6种配色任选（橙红蓝绿青蓝）。电子资料，发出不退换，建议下单前仔细考虑。【付款后自动秒发货】</t>
+          <t>大学生职业生涯规划大赛职规赛PPT模板书成长就业赛道高级感红色
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+宝贝秒拍秒发，拍下全发！你想要各种素材都在这里 任何不满意直接退款！！！
+如果没有及时回复可以先拍下来看是否需要和满意，不满意没有需要直接退款即可，上线会立即处理，您放心。
+预览图对应相应源文件名字，不是卖图片，也没有任何额外费用，如果不会使用可以咨询解决
+每套风格的模版都是我精心挑选出来的。
+每款精选质量高，适用于任何场合～
+每个风格都有单独归类文档编号
+</t>
         </is>
       </c>
       <c r="F38" s="2" t="str">
-        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i3/O1CN01lqEuk31IFlGuxBV1b_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i3/O1CN01lqEuk31IFlGuxBV1b_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp")</f>
-        <v>img.alicdn.com/bao/uploaded/i3/O1CN01lqEuk31IFlGuxBV1b_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp</v>
+        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i3/O1CN01nILD4o1dZ5wwxYefP_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i3/O1CN01nILD4o1dZ5wwxYefP_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp")</f>
+        <v>img.alicdn.com/bao/uploaded/i3/O1CN01nILD4o1dZ5wwxYefP_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp</v>
       </c>
       <c r="G38"/>
       <c r="H38" s="2" t="str">
-        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.15.69b752f39oihHY&amp;id=947881023894&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.15.69b752f39oihHY&amp;id=947881023894&amp;categoryId=50023914")</f>
-        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.15.69b752f39oihHY&amp;id=947881023894&amp;categoryId=50023914</v>
+        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.109.12e16ac2PYxLX9&amp;id=987781883336&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.109.12e16ac2PYxLX9&amp;id=987781883336&amp;categoryId=50023914")</f>
+        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.109.12e16ac2PYxLX9&amp;id=987781883336&amp;categoryId=50023914</v>
       </c>
       <c r="I38"/>
       <c r="J38"/>
@@ -2049,42 +2069,38 @@
     <row r="39" ht="25.5" customHeight="1">
       <c r="A39" t="inlineStr">
         <is>
-          <t>⚠️科研学术答辩PP</t>
+          <t>100页高级感商务大</t>
         </is>
       </c>
       <c r="B39">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>⚠️科研学术答辩PPT、毕业答辩PPT（四种配色全发，支持一|||
-键换色）
-[闪亮]ppt模版适用范围：国自然基金答辩、重点项目申报答辩、青年科学基金答辩、科研学术项目申报答辩、职称晋升答辩、学术论坛会议汇报、组会文献汇报答辩、开题答辩、中期答辩、毕业答辩等，工作汇报、路演汇报等。。
-[蓝圆]国自然基金答辩模版ppt，精美版专业汇报
-[绿圆]组会文献汇报模版ppt，秒胜同门师兄妹
-[红圆]本科、硕士、博士全领域专属答辩ppt模版
-[黄圆]科研、学术论坛汇报ppt模版，尽显专业
-[火]职称晋升、重点实验室申报答辩ppt模版
-[1]支持一键换色
-[2]蓝色、绿色、红色、紫色四种配色全发
-[3]ppt内所有元素均可自由编辑
-～ 所见即所得 ～
-需要可以直接拍下，看到马上发货哦
-❤️❤️❤️自动发货，标价就是卖价，需要直接拍，24小时秒发网盘链接
-[钉子]任何情况，不要申请退款，私信沟通给你处理，小店经营不易。
-[钉子]所有文件均获取自网络公开渠道，仅供学习和交流使用，所有版权归版权人所有，如版权方认为侵犯了您的版权，请及时联系小店删除。</t>
+          <t>100页高级感商务大气版式多图片排版图文工作总结汇报动态ppt模板
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+1款(4色)高级感图表PPT共100页
+宝贝秒拍秒发，拍下全发！你想要各种素材都在这里 任何不满意直接退款！！！
+如果没有及时回复可以先拍下来看是否需要和满意，不满意没有需要直接退款即可，上线会立即处理，您放心。
+预览图对应相应源文件名字，不是卖图片，也没有任何额外费用，如果不会使用可以咨询解决
+每套风格的模版都是我精心挑选出来的。
+每款精选质量高，适用于任何场合～
+每个风格都有单独归类文档编号
+</t>
         </is>
       </c>
       <c r="F39" s="2" t="str">
-        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i2/O1CN01dmg1R21IFlIK5Cisb_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i2/O1CN01dmg1R21IFlIK5Cisb_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp")</f>
-        <v>img.alicdn.com/bao/uploaded/i2/O1CN01dmg1R21IFlIK5Cisb_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp</v>
+        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i3/O1CN01OscPje1dZ5wkQSRoe_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i3/O1CN01OscPje1dZ5wkQSRoe_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp")</f>
+        <v>img.alicdn.com/bao/uploaded/i3/O1CN01OscPje1dZ5wkQSRoe_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp</v>
       </c>
       <c r="G39"/>
       <c r="H39" s="2" t="str">
-        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.203.69b752f39oihHY&amp;id=981387590436&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.203.69b752f39oihHY&amp;id=981387590436&amp;categoryId=50023914")</f>
-        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.203.69b752f39oihHY&amp;id=981387590436&amp;categoryId=50023914</v>
+        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.520.12e16ac2PYxLX9&amp;id=984361009829&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.520.12e16ac2PYxLX9&amp;id=984361009829&amp;categoryId=50023914")</f>
+        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.520.12e16ac2PYxLX9&amp;id=984361009829&amp;categoryId=50023914</v>
       </c>
       <c r="I39"/>
       <c r="J39"/>
@@ -2093,40 +2109,85 @@
     <row r="40" ht="25.5" customHeight="1">
       <c r="A40" t="inlineStr">
         <is>
-          <t>序言PPT模板自动秒</t>
+          <t>企业宣传册模板wor</t>
         </is>
       </c>
       <c r="B40">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>序言PPT模板自动秒发【自动秒发】序言 PPT 同款领导都爱用的 ppt 模板 工|||
-【自动秒发】序言 PPT 同款领导都爱用的 ppt 模板 工作汇报 转正述职 年终述职PPT模板 有逻辑图 240 页 持续更新～
-标价就是卖价
-数据图甘特图等各种展示模板
-下单需知：
-1.PPT 模版共计 240 页</t>
+          <t>企业宣传册模板word商务公司简介产品手画册CDR排版PSD设计AI素材
+——★24小时自动秒发百度网盘 ★——
+9999套宣传画册PSD/AI/CDR/WORD分层高清素材
+宝贝秒拍秒发，如果没有及时回复可以先拍下来看是否需要和满意，不满意没有需要直接退款即可，上线会立即处理，您放心。
+预览图对应相应源文件名字，不是卖图片，也没有任何额外费用，如果不会使用可以咨询解决
+每套风格的模版都是我精心挑选出来的。
+每款精选质量高，适用于任何场合～
+每个风格都有单独归类文档编号
+你想要 各种素材都在这里 任何不满意直接退款！！！
+</t>
         </is>
       </c>
       <c r="F40" s="2" t="str">
-        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i3/O1CN01uq4nPD1IFlGQ3DK7n_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i3/O1CN01uq4nPD1IFlGQ3DK7n_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp")</f>
-        <v>img.alicdn.com/bao/uploaded/i3/O1CN01uq4nPD1IFlGQ3DK7n_!!4611686018427383856-53-fleamarket.heic_790x10000Q90.jpg_.webp</v>
+        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i1/O1CN01cfBJJb1dZ5wElUGf4_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i1/O1CN01cfBJJb1dZ5wElUGf4_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp")</f>
+        <v>img.alicdn.com/bao/uploaded/i1/O1CN01cfBJJb1dZ5wElUGf4_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp</v>
       </c>
       <c r="G40"/>
       <c r="H40" s="2" t="str">
-        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.49.69b752f39oihHY&amp;id=936353234821&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.49.69b752f39oihHY&amp;id=936353234821&amp;categoryId=50023914")</f>
-        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.49.69b752f39oihHY&amp;id=936353234821&amp;categoryId=50023914</v>
+        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.279.12e16ac2PYxLX9&amp;id=971315835141&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.279.12e16ac2PYxLX9&amp;id=971315835141&amp;categoryId=50023914")</f>
+        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.279.12e16ac2PYxLX9&amp;id=971315835141&amp;categoryId=50023914</v>
       </c>
       <c r="I40"/>
       <c r="J40"/>
       <c r="K40"/>
     </row>
+    <row r="41" ht="25.5" customHeight="1">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025新款CAD图</t>
+        </is>
+      </c>
+      <c r="B41">
+        <v>70</v>
+      </c>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2025新款CAD图库室内设计家装家具平面中式欧式施工图动态素材库
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+——★24小时自动秒发百度网盘 ★——
+室内设计CAD图库欧式/中式/现代 赠:动态图库
+家装+工装+平面+立面+动态
+宝贝秒拍秒发，拍下全发！你想要各种素材都在这里 任何不满意直接退款！！！
+如果没有及时回复可以先拍下来看是否需要和满意，不满意没有需要直接退款即可，上线会立即处理，您放心。
+预览图对应相应源文件名字，不是卖图片，也没有任何额外费用，如果不会使用可以咨询解决
+每套风格的模版都是我精心挑选出来的。
+每款精选质量高，适用于任何场合～
+每个风格都有单独归类文档编号
+</t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="str">
+        <f>=HYPERLINK("http://img.alicdn.com/bao/uploaded/i2/O1CN01iM0BpW1dZ5x4YdUaj_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp", "img.alicdn.com/bao/uploaded/i2/O1CN01iM0BpW1dZ5x4YdUaj_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp")</f>
+        <v>img.alicdn.com/bao/uploaded/i2/O1CN01iM0BpW1dZ5x4YdUaj_!!4611686018427387605-0-fleamarket.jpg_790x10000Q90.jpg_.webp</v>
+      </c>
+      <c r="G41"/>
+      <c r="H41" s="2" t="str">
+        <f>=HYPERLINK("https://www.goofish.com/item?spm=a21ybx.personal.feeds.349.12e16ac2PYxLX9&amp;id=991568744881&amp;categoryId=50023914", "https://www.goofish.com/item?spm=a21ybx.personal.feeds.349.12e16ac2PYxLX9&amp;id=991568744881&amp;categoryId=50023914")</f>
+        <v>https://www.goofish.com/item?spm=a21ybx.personal.feeds.349.12e16ac2PYxLX9&amp;id=991568744881&amp;categoryId=50023914</v>
+      </c>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="false" sqref="C2:C39" type="list">
+    <dataValidation allowBlank="false" sqref="C2:C40" type="list">
       <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>